<commit_message>
Add study characterstics table 1 to model doc.
</commit_message>
<xml_diff>
--- a/docs/model-doc/tables-raw/studychars.xlsx
+++ b/docs/model-doc/tables-raw/studychars.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27729"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14520" tabRatio="500" firstSheet="1" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14520" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="studychar-1-1L" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="908" uniqueCount="293">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="918" uniqueCount="303">
   <si>
     <t>trial_id</t>
   </si>
@@ -1377,6 +1377,36 @@
   </si>
   <si>
     <t xml:space="preserve">Reasons for missing HRQoL data were not recorded. All other missing data balanced across groups and reasons similar. </t>
+  </si>
+  <si>
+    <t>March, 2019</t>
+  </si>
+  <si>
+    <t>June, 2019</t>
+  </si>
+  <si>
+    <t>March, 2017</t>
+  </si>
+  <si>
+    <t>November, 2017</t>
+  </si>
+  <si>
+    <t>May, 2018</t>
+  </si>
+  <si>
+    <t>January, 2024</t>
+  </si>
+  <si>
+    <t>November, 2018</t>
+  </si>
+  <si>
+    <t>December, 2018</t>
+  </si>
+  <si>
+    <t>n_1</t>
+  </si>
+  <si>
+    <t>n_2</t>
   </si>
 </sst>
 </file>
@@ -1425,8 +1455,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="19">
+  <cellStyleXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1454,7 +1486,7 @@
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="19">
+  <cellStyles count="21">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1464,6 +1496,7 @@
     <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1473,6 +1506,7 @@
     <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1805,7 +1839,7 @@
   <dimension ref="A1:R15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="Q1" sqref="Q1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0"/>
@@ -1836,10 +1870,10 @@
         <v>7</v>
       </c>
       <c r="I1" t="s">
-        <v>6</v>
+        <v>301</v>
       </c>
       <c r="J1" t="s">
-        <v>7</v>
+        <v>302</v>
       </c>
       <c r="K1" t="s">
         <v>8</v>
@@ -1900,8 +1934,8 @@
       <c r="K2" t="s">
         <v>23</v>
       </c>
-      <c r="L2" s="1">
-        <v>43553</v>
+      <c r="L2" s="1" t="s">
+        <v>293</v>
       </c>
       <c r="M2" t="s">
         <v>24</v>
@@ -2124,8 +2158,8 @@
       <c r="K6" t="s">
         <v>54</v>
       </c>
-      <c r="L6" s="1">
-        <v>43644</v>
+      <c r="L6" s="1" t="s">
+        <v>294</v>
       </c>
       <c r="M6" t="s">
         <v>24</v>
@@ -2295,8 +2329,8 @@
       <c r="L9" t="s">
         <v>24</v>
       </c>
-      <c r="M9" s="1">
-        <v>42810</v>
+      <c r="M9" s="1" t="s">
+        <v>295</v>
       </c>
       <c r="N9" t="s">
         <v>25</v>
@@ -2351,8 +2385,8 @@
       <c r="L10" t="s">
         <v>24</v>
       </c>
-      <c r="M10" s="1">
-        <v>43065</v>
+      <c r="M10" s="1" t="s">
+        <v>296</v>
       </c>
       <c r="N10" t="s">
         <v>25</v>
@@ -2407,8 +2441,8 @@
       <c r="L11" t="s">
         <v>24</v>
       </c>
-      <c r="M11" s="1">
-        <v>43251</v>
+      <c r="M11" s="1" t="s">
+        <v>297</v>
       </c>
       <c r="N11" t="s">
         <v>25</v>
@@ -2664,8 +2698,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="R4" sqref="R4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2696,10 +2730,10 @@
         <v>7</v>
       </c>
       <c r="I1" t="s">
-        <v>6</v>
+        <v>301</v>
       </c>
       <c r="J1" t="s">
-        <v>7</v>
+        <v>302</v>
       </c>
       <c r="K1" t="s">
         <v>8</v>
@@ -2754,14 +2788,11 @@
       <c r="I2">
         <v>411</v>
       </c>
-      <c r="J2" t="s">
-        <v>24</v>
-      </c>
       <c r="K2" t="s">
         <v>63</v>
       </c>
-      <c r="L2" s="3">
-        <v>45292</v>
+      <c r="L2" s="3" t="s">
+        <v>298</v>
       </c>
       <c r="M2" t="s">
         <v>24</v>
@@ -2776,6 +2807,9 @@
         <v>27</v>
       </c>
       <c r="Q2" t="s">
+        <v>24</v>
+      </c>
+      <c r="R2" t="s">
         <v>24</v>
       </c>
     </row>
@@ -2813,8 +2847,8 @@
       <c r="K3" t="s">
         <v>127</v>
       </c>
-      <c r="L3" s="3">
-        <v>43434</v>
+      <c r="L3" s="3" t="s">
+        <v>299</v>
       </c>
       <c r="M3" t="s">
         <v>24</v>
@@ -2830,6 +2864,9 @@
       </c>
       <c r="Q3" t="s">
         <v>129</v>
+      </c>
+      <c r="R3" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:18">
@@ -2866,8 +2903,8 @@
       <c r="K4" t="s">
         <v>133</v>
       </c>
-      <c r="L4" s="3">
-        <v>43465</v>
+      <c r="L4" s="3" t="s">
+        <v>300</v>
       </c>
       <c r="M4" t="s">
         <v>24</v>
@@ -2884,9 +2921,13 @@
       <c r="Q4" t="s">
         <v>136</v>
       </c>
+      <c r="R4" t="s">
+        <v>24</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -2899,9 +2940,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0"/>
   <sheetData>
@@ -4004,7 +4043,7 @@
   <dimension ref="A1:O15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -4733,7 +4772,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Complete study characteristics tables.
</commit_message>
<xml_diff>
--- a/docs/model-doc/tables-raw/studychars.xlsx
+++ b/docs/model-doc/tables-raw/studychars.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27729"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14520" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14520" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="studychar-1-1L" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="918" uniqueCount="303">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="937" uniqueCount="303">
   <si>
     <t>trial_id</t>
   </si>
@@ -468,9 +468,6 @@
   </si>
   <si>
     <t>prior_treatment_lines</t>
-  </si>
-  <si>
-    <t>prior_eggf_tki_treatment_lines</t>
   </si>
   <si>
     <t>prior_chemo_line</t>
@@ -523,9 +520,6 @@
 laboratory confirmation of an EGFR activating mutation.</t>
   </si>
   <si>
-    <t>at least 18 years (at least 20 years in Japan and South Korea)</t>
-  </si>
-  <si>
     <t>IIIb or IV</t>
   </si>
   <si>
@@ -571,9 +565,6 @@
 eligible.</t>
   </si>
   <si>
-    <t>at least 18 years</t>
-  </si>
-  <si>
     <t>0-2 (ECOG)</t>
   </si>
   <si>
@@ -603,9 +594,6 @@
 adjuvant chemotherapy was allowed if it ended Š_Ç6 months
 before entry to study). Patients with asymptomatic, stable
 brain metastases were eligible for inclusion.</t>
-  </si>
-  <si>
-    <t>greater than 18 years</t>
   </si>
   <si>
     <t>Exclusion criteria:
@@ -631,10 +619,6 @@
 Absolute contraindication for steroids.
 Dementia or significant mental disorder interfering the understanding and giving the informed consent.
 History of other malignancy except adequately treated basal cell or squamous cell skin cancer, carcinoma in situ of the cervix, radically treated prostatic carcinoma with good prognostic (Gleason = 6). History of other curatively treated malignancy and no evidence of disease within the past 5 years.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">No. Patients with asymptomatic brain metastasis and stable with medical treatment will be eligible for the study. Patients having received radiotherapy for their brain metastasis prior to the systemic treatment for the NSCLC will be also eligible.
-</t>
   </si>
   <si>
     <t>All tissue samples were analysed with Sanger
@@ -1107,9 +1091,6 @@
 Females of child-bearing potential using contraception; negative pregnancy test.</t>
   </si>
   <si>
-    <t>At least 18 years (at least 20 years in Japan)</t>
-  </si>
-  <si>
     <t>At least 12 weeks</t>
   </si>
   <si>
@@ -1147,9 +1128,6 @@
 metastases that had not been treated with glucocorticoids
 for at least 4 weeks before the first
 dose of a trial drug were eligible for inclusion.</t>
-  </si>
-  <si>
-    <t>At least 18 years</t>
   </si>
   <si>
     <t>1. Treatment with any of the following:
@@ -1181,9 +1159,6 @@
 absorption of AZD9291.</t>
   </si>
   <si>
-    <t xml:space="preserve">Yes unless asymptomatic, stable and not requiring steroids. </t>
-  </si>
-  <si>
     <t>Cobas EGFR Mutation Test (Roche) version 2</t>
   </si>
   <si>
@@ -1407,6 +1382,31 @@
   </si>
   <si>
     <t>n_2</t>
+  </si>
+  <si>
+    <t>&gt; 18 years</t>
+  </si>
+  <si>
+    <t>prior_egfr_tki_treatment_lines</t>
+  </si>
+  <si>
+    <t>$\geq$ 18</t>
+  </si>
+  <si>
+    <t>$\geq$ 18 years</t>
+  </si>
+  <si>
+    <t>$\geq$ 18 ($\geq$ 20 in Japan and South Korea)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Patients with asymptomatic brain metastasis and stable with medical treatment will be eligible for the study. Patients having received radiotherapy for their brain metastasis prior to the systemic treatment for the NSCLC will be also eligible.
+</t>
+  </si>
+  <si>
+    <t>cns_metastases_excluded_detail</t>
+  </si>
+  <si>
+    <t>$\geq$ 18 ($\geq$ 20 in Japan)</t>
   </si>
 </sst>
 </file>
@@ -1455,8 +1455,30 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="21">
+  <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1486,7 +1508,7 @@
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="21">
+  <cellStyles count="43">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1497,6 +1519,17 @@
     <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1507,6 +1540,17 @@
     <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1870,10 +1914,10 @@
         <v>7</v>
       </c>
       <c r="I1" t="s">
-        <v>301</v>
+        <v>293</v>
       </c>
       <c r="J1" t="s">
-        <v>302</v>
+        <v>294</v>
       </c>
       <c r="K1" t="s">
         <v>8</v>
@@ -1935,7 +1979,7 @@
         <v>23</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>293</v>
+        <v>285</v>
       </c>
       <c r="M2" t="s">
         <v>24</v>
@@ -2159,7 +2203,7 @@
         <v>54</v>
       </c>
       <c r="L6" s="1" t="s">
-        <v>294</v>
+        <v>286</v>
       </c>
       <c r="M6" t="s">
         <v>24</v>
@@ -2330,7 +2374,7 @@
         <v>24</v>
       </c>
       <c r="M9" s="1" t="s">
-        <v>295</v>
+        <v>287</v>
       </c>
       <c r="N9" t="s">
         <v>25</v>
@@ -2386,7 +2430,7 @@
         <v>24</v>
       </c>
       <c r="M10" s="1" t="s">
-        <v>296</v>
+        <v>288</v>
       </c>
       <c r="N10" t="s">
         <v>25</v>
@@ -2442,7 +2486,7 @@
         <v>24</v>
       </c>
       <c r="M11" s="1" t="s">
-        <v>297</v>
+        <v>289</v>
       </c>
       <c r="N11" t="s">
         <v>25</v>
@@ -2698,7 +2742,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+    <sheetView topLeftCell="C1" workbookViewId="0">
       <selection activeCell="R4" sqref="R4"/>
     </sheetView>
   </sheetViews>
@@ -2730,10 +2774,10 @@
         <v>7</v>
       </c>
       <c r="I1" t="s">
-        <v>301</v>
+        <v>293</v>
       </c>
       <c r="J1" t="s">
-        <v>302</v>
+        <v>294</v>
       </c>
       <c r="K1" t="s">
         <v>8</v>
@@ -2792,7 +2836,7 @@
         <v>63</v>
       </c>
       <c r="L2" s="3" t="s">
-        <v>298</v>
+        <v>290</v>
       </c>
       <c r="M2" t="s">
         <v>24</v>
@@ -2848,7 +2892,7 @@
         <v>127</v>
       </c>
       <c r="L3" s="3" t="s">
-        <v>299</v>
+        <v>291</v>
       </c>
       <c r="M3" t="s">
         <v>24</v>
@@ -2904,7 +2948,7 @@
         <v>133</v>
       </c>
       <c r="L4" s="3" t="s">
-        <v>300</v>
+        <v>292</v>
       </c>
       <c r="M4" t="s">
         <v>24</v>
@@ -2938,13 +2982,15 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R15"/>
+  <dimension ref="A1:S15"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:18" ht="15" customHeight="1">
+    <row r="1" spans="1:19" ht="15" customHeight="1">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2979,154 +3025,163 @@
         <v>146</v>
       </c>
       <c r="L1" t="s">
+        <v>296</v>
+      </c>
+      <c r="M1" t="s">
         <v>147</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>148</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>149</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>150</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>151</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
+        <v>301</v>
+      </c>
+      <c r="S1" t="s">
         <v>152</v>
       </c>
-      <c r="R1" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="2" spans="1:18" ht="15" customHeight="1">
+    </row>
+    <row r="2" spans="1:19" ht="15" customHeight="1">
       <c r="A2" t="s">
         <v>16</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="C2" t="s">
+        <v>299</v>
+      </c>
+      <c r="D2" t="s">
         <v>154</v>
       </c>
-      <c r="C2" t="s">
+      <c r="E2" t="s">
         <v>155</v>
       </c>
-      <c r="D2" t="s">
+      <c r="F2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G2" t="s">
         <v>156</v>
       </c>
-      <c r="E2" t="s">
+      <c r="H2" t="s">
+        <v>24</v>
+      </c>
+      <c r="I2" t="s">
+        <v>24</v>
+      </c>
+      <c r="J2" t="s">
         <v>157</v>
       </c>
-      <c r="F2" t="s">
-        <v>24</v>
-      </c>
-      <c r="G2" t="s">
+      <c r="K2" t="s">
+        <v>28</v>
+      </c>
+      <c r="L2" t="s">
+        <v>28</v>
+      </c>
+      <c r="M2" t="s">
+        <v>28</v>
+      </c>
+      <c r="N2" t="s">
+        <v>28</v>
+      </c>
+      <c r="O2" s="2" t="s">
         <v>158</v>
       </c>
-      <c r="H2" t="s">
-        <v>24</v>
-      </c>
-      <c r="I2" t="s">
-        <v>24</v>
-      </c>
-      <c r="J2" t="s">
+      <c r="P2" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>27</v>
+      </c>
+      <c r="R2" t="s">
+        <v>27</v>
+      </c>
+      <c r="S2" s="2" t="s">
         <v>159</v>
       </c>
-      <c r="K2" t="s">
-        <v>28</v>
-      </c>
-      <c r="L2" t="s">
-        <v>28</v>
-      </c>
-      <c r="M2" t="s">
-        <v>28</v>
-      </c>
-      <c r="N2" t="s">
-        <v>28</v>
-      </c>
-      <c r="O2" s="2" t="s">
-        <v>160</v>
-      </c>
-      <c r="P2" t="s">
-        <v>27</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>27</v>
-      </c>
-      <c r="R2" s="2" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="3" spans="1:18" ht="15" customHeight="1">
+    </row>
+    <row r="3" spans="1:19" ht="15" customHeight="1">
       <c r="A3" t="s">
         <v>29</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="C3" t="s">
+        <v>297</v>
+      </c>
+      <c r="D3" t="s">
+        <v>154</v>
+      </c>
+      <c r="E3" t="s">
+        <v>161</v>
+      </c>
+      <c r="F3" t="s">
+        <v>24</v>
+      </c>
+      <c r="G3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H3" t="s">
+        <v>24</v>
+      </c>
+      <c r="I3" t="s">
         <v>162</v>
       </c>
-      <c r="C3" t="s">
+      <c r="J3" t="s">
         <v>163</v>
       </c>
-      <c r="D3" t="s">
-        <v>156</v>
-      </c>
-      <c r="E3" t="s">
+      <c r="K3" t="s">
+        <v>28</v>
+      </c>
+      <c r="L3" t="s">
+        <v>28</v>
+      </c>
+      <c r="M3" t="s">
+        <v>28</v>
+      </c>
+      <c r="N3" t="s">
+        <v>28</v>
+      </c>
+      <c r="O3" s="2" t="s">
         <v>164</v>
       </c>
-      <c r="F3" t="s">
-        <v>24</v>
-      </c>
-      <c r="G3" t="s">
-        <v>24</v>
-      </c>
-      <c r="H3" t="s">
-        <v>24</v>
-      </c>
-      <c r="I3" t="s">
+      <c r="P3" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>27</v>
+      </c>
+      <c r="R3" t="s">
+        <v>27</v>
+      </c>
+      <c r="S3" s="2" t="s">
         <v>165</v>
       </c>
-      <c r="J3" t="s">
-        <v>166</v>
-      </c>
-      <c r="K3" t="s">
-        <v>28</v>
-      </c>
-      <c r="L3" t="s">
-        <v>28</v>
-      </c>
-      <c r="M3" t="s">
-        <v>28</v>
-      </c>
-      <c r="N3" t="s">
-        <v>28</v>
-      </c>
-      <c r="O3" s="2" t="s">
-        <v>167</v>
-      </c>
-      <c r="P3" t="s">
-        <v>27</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>27</v>
-      </c>
-      <c r="R3" s="2" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="4" spans="1:18" ht="15" customHeight="1">
+    </row>
+    <row r="4" spans="1:19" ht="15" customHeight="1">
       <c r="A4" t="s">
         <v>37</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="C4" t="s">
-        <v>170</v>
+        <v>295</v>
       </c>
       <c r="D4" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="E4" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="F4" t="s">
         <v>24</v>
@@ -3141,7 +3196,7 @@
         <v>24</v>
       </c>
       <c r="J4" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="K4" t="s">
         <v>28</v>
@@ -3156,45 +3211,48 @@
         <v>28</v>
       </c>
       <c r="O4" s="2" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="P4" t="s">
         <v>27</v>
       </c>
-      <c r="Q4" s="2" t="s">
-        <v>172</v>
+      <c r="Q4" t="s">
+        <v>28</v>
       </c>
       <c r="R4" s="2" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="5" spans="1:18" ht="15" customHeight="1">
+        <v>300</v>
+      </c>
+      <c r="S4" s="2" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" ht="15" customHeight="1">
       <c r="A5" t="s">
         <v>45</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="C5" t="s">
+        <v>295</v>
+      </c>
+      <c r="D5" t="s">
+        <v>154</v>
+      </c>
+      <c r="E5" t="s">
+        <v>161</v>
+      </c>
+      <c r="F5" t="s">
+        <v>24</v>
+      </c>
+      <c r="G5" t="s">
+        <v>156</v>
+      </c>
+      <c r="H5" t="s">
         <v>170</v>
       </c>
-      <c r="D5" t="s">
-        <v>156</v>
-      </c>
-      <c r="E5" t="s">
-        <v>164</v>
-      </c>
-      <c r="F5" t="s">
-        <v>24</v>
-      </c>
-      <c r="G5" t="s">
-        <v>158</v>
-      </c>
-      <c r="H5" t="s">
-        <v>175</v>
-      </c>
       <c r="I5" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="J5" t="s">
         <v>24</v>
@@ -3212,104 +3270,110 @@
         <v>28</v>
       </c>
       <c r="O5" s="2" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="P5" t="s">
         <v>27</v>
       </c>
       <c r="Q5" t="s">
-        <v>177</v>
-      </c>
-      <c r="R5" s="2" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="6" spans="1:18" ht="15" customHeight="1">
+        <v>27</v>
+      </c>
+      <c r="R5" t="s">
+        <v>172</v>
+      </c>
+      <c r="S5" s="2" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" ht="15" customHeight="1">
       <c r="A6" t="s">
         <v>49</v>
       </c>
       <c r="B6" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="C6" t="s">
+        <v>298</v>
+      </c>
+      <c r="D6" t="s">
+        <v>154</v>
+      </c>
+      <c r="E6" t="s">
+        <v>175</v>
+      </c>
+      <c r="F6" t="s">
+        <v>176</v>
+      </c>
+      <c r="G6" t="s">
+        <v>156</v>
+      </c>
+      <c r="H6" t="s">
+        <v>24</v>
+      </c>
+      <c r="I6" t="s">
+        <v>24</v>
+      </c>
+      <c r="J6" t="s">
+        <v>177</v>
+      </c>
+      <c r="K6" t="s">
+        <v>28</v>
+      </c>
+      <c r="L6" t="s">
+        <v>28</v>
+      </c>
+      <c r="M6" t="s">
+        <v>28</v>
+      </c>
+      <c r="N6" t="s">
+        <v>28</v>
+      </c>
+      <c r="O6" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="P6" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>28</v>
+      </c>
+      <c r="R6" t="s">
         <v>179</v>
       </c>
-      <c r="C6" t="s">
-        <v>163</v>
-      </c>
-      <c r="D6" t="s">
-        <v>156</v>
-      </c>
-      <c r="E6" t="s">
+      <c r="S6" t="s">
         <v>180</v>
       </c>
-      <c r="F6" t="s">
-        <v>181</v>
-      </c>
-      <c r="G6" t="s">
-        <v>158</v>
-      </c>
-      <c r="H6" t="s">
-        <v>24</v>
-      </c>
-      <c r="I6" t="s">
-        <v>24</v>
-      </c>
-      <c r="J6" t="s">
-        <v>182</v>
-      </c>
-      <c r="K6" t="s">
-        <v>28</v>
-      </c>
-      <c r="L6" t="s">
-        <v>28</v>
-      </c>
-      <c r="M6" t="s">
-        <v>28</v>
-      </c>
-      <c r="N6" t="s">
-        <v>28</v>
-      </c>
-      <c r="O6" s="2" t="s">
-        <v>183</v>
-      </c>
-      <c r="P6" t="s">
-        <v>27</v>
-      </c>
-      <c r="Q6" t="s">
-        <v>184</v>
-      </c>
-      <c r="R6" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="7" spans="1:18" ht="15" customHeight="1">
+    </row>
+    <row r="7" spans="1:19" ht="15" customHeight="1">
       <c r="A7" t="s">
         <v>58</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
       <c r="C7" t="s">
-        <v>170</v>
+        <v>295</v>
       </c>
       <c r="D7" t="s">
+        <v>154</v>
+      </c>
+      <c r="E7" t="s">
+        <v>155</v>
+      </c>
+      <c r="F7" t="s">
+        <v>24</v>
+      </c>
+      <c r="G7" t="s">
         <v>156</v>
       </c>
-      <c r="E7" t="s">
-        <v>157</v>
-      </c>
-      <c r="F7" t="s">
-        <v>24</v>
-      </c>
-      <c r="G7" t="s">
-        <v>158</v>
-      </c>
       <c r="H7" t="s">
         <v>24</v>
       </c>
       <c r="I7" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="J7" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="K7" t="s">
         <v>28</v>
@@ -3324,7 +3388,7 @@
         <v>28</v>
       </c>
       <c r="O7" s="2" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="P7" t="s">
         <v>27</v>
@@ -3333,36 +3397,39 @@
         <v>27</v>
       </c>
       <c r="R7" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="8" spans="1:18" ht="15" customHeight="1">
+        <v>27</v>
+      </c>
+      <c r="S7" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" ht="15" customHeight="1">
       <c r="A8" t="s">
         <v>67</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="C8" t="s">
-        <v>163</v>
+        <v>298</v>
       </c>
       <c r="D8" t="s">
+        <v>154</v>
+      </c>
+      <c r="E8" t="s">
+        <v>186</v>
+      </c>
+      <c r="F8" t="s">
+        <v>24</v>
+      </c>
+      <c r="G8" t="s">
         <v>156</v>
       </c>
-      <c r="E8" t="s">
-        <v>191</v>
-      </c>
-      <c r="F8" t="s">
-        <v>24</v>
-      </c>
-      <c r="G8" t="s">
-        <v>158</v>
-      </c>
       <c r="H8" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="I8" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="J8" t="s">
         <v>24</v>
@@ -3380,7 +3447,7 @@
         <v>28</v>
       </c>
       <c r="O8" s="2" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="P8" t="s">
         <v>27</v>
@@ -3389,31 +3456,34 @@
         <v>24</v>
       </c>
       <c r="R8" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="9" spans="1:18" ht="15" customHeight="1">
+        <v>24</v>
+      </c>
+      <c r="S8" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" ht="15" customHeight="1">
       <c r="A9" t="s">
         <v>75</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="C9" t="s">
-        <v>163</v>
+        <v>295</v>
       </c>
       <c r="D9" t="s">
+        <v>154</v>
+      </c>
+      <c r="E9" t="s">
+        <v>155</v>
+      </c>
+      <c r="F9" t="s">
+        <v>176</v>
+      </c>
+      <c r="G9" t="s">
         <v>156</v>
       </c>
-      <c r="E9" t="s">
-        <v>157</v>
-      </c>
-      <c r="F9" t="s">
-        <v>181</v>
-      </c>
-      <c r="G9" t="s">
-        <v>158</v>
-      </c>
       <c r="H9" t="s">
         <v>24</v>
       </c>
@@ -3421,7 +3491,7 @@
         <v>24</v>
       </c>
       <c r="J9" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="K9" t="s">
         <v>28</v>
@@ -3436,64 +3506,67 @@
         <v>28</v>
       </c>
       <c r="O9" s="2" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="P9" t="s">
         <v>27</v>
       </c>
       <c r="Q9" t="s">
-        <v>198</v>
-      </c>
-      <c r="R9" s="2" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="10" spans="1:18" ht="15" customHeight="1">
+        <v>27</v>
+      </c>
+      <c r="R9" t="s">
+        <v>193</v>
+      </c>
+      <c r="S9" s="2" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" ht="15" customHeight="1">
       <c r="A10" t="s">
         <v>83</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="C10" t="s">
-        <v>163</v>
+        <v>298</v>
       </c>
       <c r="D10" t="s">
+        <v>154</v>
+      </c>
+      <c r="E10" t="s">
+        <v>155</v>
+      </c>
+      <c r="F10" t="s">
+        <v>176</v>
+      </c>
+      <c r="G10" t="s">
         <v>156</v>
       </c>
-      <c r="E10" t="s">
-        <v>157</v>
-      </c>
-      <c r="F10" t="s">
-        <v>181</v>
-      </c>
-      <c r="G10" t="s">
-        <v>158</v>
-      </c>
       <c r="H10" t="s">
         <v>24</v>
       </c>
       <c r="I10" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="J10" t="s">
+        <v>191</v>
+      </c>
+      <c r="K10" t="s">
+        <v>28</v>
+      </c>
+      <c r="L10" t="s">
+        <v>28</v>
+      </c>
+      <c r="M10" t="s">
+        <v>28</v>
+      </c>
+      <c r="N10" t="s">
+        <v>28</v>
+      </c>
+      <c r="O10" s="2" t="s">
         <v>196</v>
       </c>
-      <c r="K10" t="s">
-        <v>28</v>
-      </c>
-      <c r="L10" t="s">
-        <v>28</v>
-      </c>
-      <c r="M10" t="s">
-        <v>28</v>
-      </c>
-      <c r="N10" t="s">
-        <v>28</v>
-      </c>
-      <c r="O10" s="2" t="s">
-        <v>201</v>
-      </c>
       <c r="P10" t="s">
         <v>27</v>
       </c>
@@ -3501,31 +3574,34 @@
         <v>27</v>
       </c>
       <c r="R10" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="11" spans="1:18" ht="15" customHeight="1">
+        <v>27</v>
+      </c>
+      <c r="S10" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" ht="15" customHeight="1">
       <c r="A11" t="s">
         <v>87</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="C11" t="s">
-        <v>163</v>
+        <v>298</v>
       </c>
       <c r="D11" t="s">
+        <v>154</v>
+      </c>
+      <c r="E11" t="s">
+        <v>155</v>
+      </c>
+      <c r="F11" t="s">
+        <v>24</v>
+      </c>
+      <c r="G11" t="s">
         <v>156</v>
       </c>
-      <c r="E11" t="s">
-        <v>157</v>
-      </c>
-      <c r="F11" t="s">
-        <v>24</v>
-      </c>
-      <c r="G11" t="s">
-        <v>158</v>
-      </c>
       <c r="H11" t="s">
         <v>24</v>
       </c>
@@ -3533,7 +3609,7 @@
         <v>24</v>
       </c>
       <c r="J11" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="K11" t="s">
         <v>28</v>
@@ -3548,36 +3624,39 @@
         <v>28</v>
       </c>
       <c r="O11" s="2" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="P11" t="s">
         <v>27</v>
       </c>
       <c r="Q11" t="s">
-        <v>205</v>
+        <v>27</v>
       </c>
       <c r="R11" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="12" spans="1:18" ht="15" customHeight="1">
+        <v>200</v>
+      </c>
+      <c r="S11" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" ht="15" customHeight="1">
       <c r="A12" t="s">
         <v>93</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="C12" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="D12" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="E12" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="F12" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="G12" t="s">
         <v>24</v>
@@ -3586,10 +3665,10 @@
         <v>24</v>
       </c>
       <c r="I12" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="J12" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="K12" t="s">
         <v>28</v>
@@ -3604,36 +3683,39 @@
         <v>28</v>
       </c>
       <c r="O12" s="2" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="P12" t="s">
         <v>27</v>
       </c>
       <c r="Q12" t="s">
-        <v>210</v>
+        <v>27</v>
       </c>
       <c r="R12" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="13" spans="1:18" ht="15" customHeight="1">
+        <v>205</v>
+      </c>
+      <c r="S12" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" ht="15" customHeight="1">
       <c r="A13" t="s">
         <v>97</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="C13" t="s">
-        <v>163</v>
+        <v>295</v>
       </c>
       <c r="D13" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="E13" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="F13" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="G13" t="s">
         <v>24</v>
@@ -3642,10 +3724,10 @@
         <v>24</v>
       </c>
       <c r="I13" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="J13" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="K13" t="s">
         <v>28</v>
@@ -3660,7 +3742,7 @@
         <v>28</v>
       </c>
       <c r="O13" s="2" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="P13" t="s">
         <v>27</v>
@@ -3669,24 +3751,27 @@
         <v>27</v>
       </c>
       <c r="R13" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="14" spans="1:18" ht="15" customHeight="1">
+        <v>27</v>
+      </c>
+      <c r="S13" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" ht="15" customHeight="1">
       <c r="A14" t="s">
         <v>104</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="C14" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="D14" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="E14" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="F14" t="s">
         <v>24</v>
@@ -3698,10 +3783,10 @@
         <v>24</v>
       </c>
       <c r="I14" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="J14" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="K14" t="s">
         <v>28</v>
@@ -3716,7 +3801,7 @@
         <v>28</v>
       </c>
       <c r="O14" s="2" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="P14" t="s">
         <v>27</v>
@@ -3724,40 +3809,43 @@
       <c r="Q14" t="s">
         <v>27</v>
       </c>
-      <c r="R14" s="2" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="15" spans="1:18" ht="15" customHeight="1">
+      <c r="R14" t="s">
+        <v>27</v>
+      </c>
+      <c r="S14" s="2" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" ht="15" customHeight="1">
       <c r="A15" t="s">
         <v>111</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="C15" t="s">
-        <v>163</v>
+        <v>298</v>
       </c>
       <c r="D15" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="E15" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="F15" t="s">
         <v>24</v>
       </c>
       <c r="G15" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
       <c r="H15" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
       <c r="I15" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="J15" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="K15" t="s">
         <v>28</v>
@@ -3772,7 +3860,7 @@
         <v>28</v>
       </c>
       <c r="O15" s="2" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
       <c r="P15" t="s">
         <v>27</v>
@@ -3780,12 +3868,16 @@
       <c r="Q15" t="s">
         <v>27</v>
       </c>
-      <c r="R15" s="2" t="s">
-        <v>223</v>
+      <c r="R15" t="s">
+        <v>27</v>
+      </c>
+      <c r="S15" s="2" t="s">
+        <v>218</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -3796,15 +3888,15 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R4"/>
+  <dimension ref="A1:S4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:18">
+    <row r="1" spans="1:19">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3839,49 +3931,52 @@
         <v>146</v>
       </c>
       <c r="L1" t="s">
+        <v>296</v>
+      </c>
+      <c r="M1" t="s">
         <v>147</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>148</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>149</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>150</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>151</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
+        <v>301</v>
+      </c>
+      <c r="S1" t="s">
         <v>152</v>
       </c>
-      <c r="R1" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="2" spans="1:18">
+    </row>
+    <row r="2" spans="1:19">
       <c r="A2" t="s">
         <v>119</v>
       </c>
       <c r="B2" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="C2" t="s">
-        <v>225</v>
+        <v>302</v>
       </c>
       <c r="D2" t="s">
+        <v>154</v>
+      </c>
+      <c r="E2" t="s">
+        <v>175</v>
+      </c>
+      <c r="F2" t="s">
+        <v>220</v>
+      </c>
+      <c r="G2" t="s">
         <v>156</v>
       </c>
-      <c r="E2" t="s">
-        <v>180</v>
-      </c>
-      <c r="F2" t="s">
-        <v>226</v>
-      </c>
-      <c r="G2" t="s">
-        <v>158</v>
-      </c>
       <c r="H2" t="s">
         <v>24</v>
       </c>
@@ -3889,7 +3984,7 @@
         <v>24</v>
       </c>
       <c r="J2" t="s">
-        <v>227</v>
+        <v>221</v>
       </c>
       <c r="K2" t="s">
         <v>27</v>
@@ -3904,33 +3999,36 @@
         <v>24</v>
       </c>
       <c r="O2" t="s">
-        <v>228</v>
+        <v>222</v>
       </c>
       <c r="P2" t="s">
         <v>28</v>
       </c>
       <c r="Q2" t="s">
-        <v>229</v>
+        <v>27</v>
       </c>
       <c r="R2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="3" spans="1:18">
+        <v>223</v>
+      </c>
+      <c r="S2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19">
       <c r="A3" t="s">
         <v>124</v>
       </c>
       <c r="B3" t="s">
-        <v>230</v>
+        <v>224</v>
       </c>
       <c r="C3" t="s">
-        <v>231</v>
+        <v>298</v>
       </c>
       <c r="D3" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="E3" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="F3" t="s">
         <v>24</v>
@@ -3945,7 +4043,7 @@
         <v>24</v>
       </c>
       <c r="J3" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="K3" t="s">
         <v>27</v>
@@ -3960,40 +4058,43 @@
         <v>28</v>
       </c>
       <c r="O3" t="s">
-        <v>232</v>
+        <v>225</v>
       </c>
       <c r="P3" t="s">
         <v>28</v>
       </c>
       <c r="Q3" t="s">
-        <v>233</v>
+        <v>27</v>
       </c>
       <c r="R3" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="4" spans="1:18">
+        <v>223</v>
+      </c>
+      <c r="S3" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19">
       <c r="A4" t="s">
         <v>130</v>
       </c>
       <c r="B4" t="s">
-        <v>235</v>
+        <v>227</v>
       </c>
       <c r="C4" t="s">
-        <v>225</v>
+        <v>302</v>
       </c>
       <c r="D4" t="s">
+        <v>154</v>
+      </c>
+      <c r="E4" t="s">
+        <v>175</v>
+      </c>
+      <c r="F4" t="s">
+        <v>220</v>
+      </c>
+      <c r="G4" t="s">
         <v>156</v>
       </c>
-      <c r="E4" t="s">
-        <v>180</v>
-      </c>
-      <c r="F4" t="s">
-        <v>226</v>
-      </c>
-      <c r="G4" t="s">
-        <v>158</v>
-      </c>
       <c r="H4" t="s">
         <v>24</v>
       </c>
@@ -4001,7 +4102,7 @@
         <v>24</v>
       </c>
       <c r="J4" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="K4" t="s">
         <v>27</v>
@@ -4016,20 +4117,24 @@
         <v>28</v>
       </c>
       <c r="O4" t="s">
-        <v>236</v>
+        <v>228</v>
       </c>
       <c r="P4" t="s">
         <v>27</v>
       </c>
       <c r="Q4" t="s">
-        <v>210</v>
+        <v>27</v>
       </c>
       <c r="R4" t="s">
-        <v>237</v>
+        <v>223</v>
+      </c>
+      <c r="S4" t="s">
+        <v>229</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -4042,8 +4147,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -4057,46 +4162,46 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>261</v>
+      </c>
+      <c r="C1" t="s">
+        <v>260</v>
+      </c>
+      <c r="D1" t="s">
+        <v>262</v>
+      </c>
+      <c r="E1" t="s">
+        <v>263</v>
+      </c>
+      <c r="F1" t="s">
+        <v>264</v>
+      </c>
+      <c r="G1" t="s">
+        <v>265</v>
+      </c>
+      <c r="H1" t="s">
+        <v>266</v>
+      </c>
+      <c r="I1" t="s">
+        <v>267</v>
+      </c>
+      <c r="J1" t="s">
+        <v>268</v>
+      </c>
+      <c r="K1" t="s">
         <v>269</v>
       </c>
-      <c r="C1" t="s">
-        <v>268</v>
-      </c>
-      <c r="D1" t="s">
+      <c r="L1" t="s">
         <v>270</v>
       </c>
-      <c r="E1" t="s">
+      <c r="M1" t="s">
         <v>271</v>
       </c>
-      <c r="F1" t="s">
+      <c r="N1" t="s">
         <v>272</v>
       </c>
-      <c r="G1" t="s">
+      <c r="O1" t="s">
         <v>273</v>
-      </c>
-      <c r="H1" t="s">
-        <v>274</v>
-      </c>
-      <c r="I1" t="s">
-        <v>275</v>
-      </c>
-      <c r="J1" t="s">
-        <v>276</v>
-      </c>
-      <c r="K1" t="s">
-        <v>277</v>
-      </c>
-      <c r="L1" t="s">
-        <v>278</v>
-      </c>
-      <c r="M1" t="s">
-        <v>279</v>
-      </c>
-      <c r="N1" t="s">
-        <v>280</v>
-      </c>
-      <c r="O1" t="s">
-        <v>281</v>
       </c>
     </row>
     <row r="2" spans="1:15">
@@ -4104,46 +4209,46 @@
         <v>16</v>
       </c>
       <c r="B2" t="s">
-        <v>238</v>
+        <v>230</v>
       </c>
       <c r="C2" t="s">
-        <v>239</v>
+        <v>231</v>
       </c>
       <c r="D2" t="s">
-        <v>238</v>
+        <v>230</v>
       </c>
       <c r="E2" t="s">
-        <v>240</v>
+        <v>232</v>
       </c>
       <c r="F2" t="s">
-        <v>241</v>
+        <v>233</v>
       </c>
       <c r="G2" t="s">
         <v>25</v>
       </c>
       <c r="H2" t="s">
-        <v>238</v>
+        <v>230</v>
       </c>
       <c r="I2" t="s">
-        <v>242</v>
+        <v>234</v>
       </c>
       <c r="J2" t="s">
-        <v>238</v>
+        <v>230</v>
       </c>
       <c r="K2" t="s">
-        <v>243</v>
+        <v>235</v>
       </c>
       <c r="L2" t="s">
-        <v>238</v>
+        <v>230</v>
       </c>
       <c r="M2" t="s">
-        <v>244</v>
+        <v>236</v>
       </c>
       <c r="N2" t="s">
-        <v>245</v>
+        <v>237</v>
       </c>
       <c r="O2" t="s">
-        <v>282</v>
+        <v>274</v>
       </c>
     </row>
     <row r="3" spans="1:15">
@@ -4151,46 +4256,46 @@
         <v>29</v>
       </c>
       <c r="B3" t="s">
+        <v>230</v>
+      </c>
+      <c r="C3" t="s">
+        <v>231</v>
+      </c>
+      <c r="D3" t="s">
         <v>238</v>
       </c>
-      <c r="C3" t="s">
+      <c r="E3" t="s">
         <v>239</v>
       </c>
-      <c r="D3" t="s">
-        <v>246</v>
-      </c>
-      <c r="E3" t="s">
-        <v>247</v>
-      </c>
       <c r="F3" t="s">
-        <v>241</v>
+        <v>233</v>
       </c>
       <c r="G3" t="s">
         <v>25</v>
       </c>
       <c r="H3" t="s">
-        <v>238</v>
+        <v>230</v>
       </c>
       <c r="I3" t="s">
-        <v>248</v>
+        <v>240</v>
       </c>
       <c r="J3" t="s">
-        <v>238</v>
+        <v>230</v>
       </c>
       <c r="K3" t="s">
-        <v>243</v>
+        <v>235</v>
       </c>
       <c r="L3" t="s">
-        <v>238</v>
+        <v>230</v>
       </c>
       <c r="M3" t="s">
-        <v>244</v>
+        <v>236</v>
       </c>
       <c r="N3" t="s">
-        <v>245</v>
+        <v>237</v>
       </c>
       <c r="O3" t="s">
-        <v>283</v>
+        <v>275</v>
       </c>
     </row>
     <row r="4" spans="1:15">
@@ -4198,46 +4303,46 @@
         <v>37</v>
       </c>
       <c r="B4" t="s">
-        <v>238</v>
+        <v>230</v>
       </c>
       <c r="C4" t="s">
-        <v>239</v>
+        <v>231</v>
       </c>
       <c r="D4" t="s">
-        <v>238</v>
+        <v>230</v>
       </c>
       <c r="E4" t="s">
-        <v>249</v>
+        <v>241</v>
       </c>
       <c r="F4" t="s">
-        <v>241</v>
+        <v>233</v>
       </c>
       <c r="G4" t="s">
         <v>25</v>
       </c>
       <c r="H4" t="s">
-        <v>238</v>
+        <v>230</v>
       </c>
       <c r="I4" t="s">
-        <v>250</v>
+        <v>242</v>
       </c>
       <c r="J4" t="s">
-        <v>238</v>
+        <v>230</v>
       </c>
       <c r="K4" t="s">
-        <v>243</v>
+        <v>235</v>
       </c>
       <c r="L4" t="s">
-        <v>238</v>
+        <v>230</v>
       </c>
       <c r="M4" t="s">
-        <v>244</v>
+        <v>236</v>
       </c>
       <c r="N4" t="s">
-        <v>245</v>
+        <v>237</v>
       </c>
       <c r="O4" t="s">
-        <v>283</v>
+        <v>275</v>
       </c>
     </row>
     <row r="5" spans="1:15">
@@ -4245,46 +4350,46 @@
         <v>45</v>
       </c>
       <c r="B5" t="s">
+        <v>230</v>
+      </c>
+      <c r="C5" t="s">
+        <v>231</v>
+      </c>
+      <c r="D5" t="s">
         <v>238</v>
       </c>
-      <c r="C5" t="s">
+      <c r="E5" t="s">
         <v>239</v>
       </c>
-      <c r="D5" t="s">
-        <v>246</v>
-      </c>
-      <c r="E5" t="s">
-        <v>247</v>
-      </c>
       <c r="F5" t="s">
-        <v>241</v>
+        <v>233</v>
       </c>
       <c r="G5" t="s">
         <v>25</v>
       </c>
       <c r="H5" t="s">
-        <v>238</v>
+        <v>230</v>
       </c>
       <c r="I5" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="J5" t="s">
-        <v>238</v>
+        <v>230</v>
       </c>
       <c r="K5" t="s">
-        <v>243</v>
+        <v>235</v>
       </c>
       <c r="L5" t="s">
-        <v>238</v>
+        <v>230</v>
       </c>
       <c r="M5" t="s">
-        <v>244</v>
+        <v>236</v>
       </c>
       <c r="N5" t="s">
-        <v>245</v>
+        <v>237</v>
       </c>
       <c r="O5" t="s">
-        <v>283</v>
+        <v>275</v>
       </c>
     </row>
     <row r="6" spans="1:15">
@@ -4292,46 +4397,46 @@
         <v>49</v>
       </c>
       <c r="B6" t="s">
-        <v>238</v>
+        <v>230</v>
       </c>
       <c r="C6" t="s">
-        <v>239</v>
+        <v>231</v>
       </c>
       <c r="D6" t="s">
-        <v>238</v>
+        <v>230</v>
       </c>
       <c r="E6" t="s">
-        <v>252</v>
+        <v>244</v>
       </c>
       <c r="F6" t="s">
-        <v>238</v>
+        <v>230</v>
       </c>
       <c r="G6" t="s">
         <v>55</v>
       </c>
       <c r="H6" t="s">
-        <v>238</v>
+        <v>230</v>
       </c>
       <c r="I6" t="s">
-        <v>253</v>
+        <v>245</v>
       </c>
       <c r="J6" t="s">
-        <v>238</v>
+        <v>230</v>
       </c>
       <c r="K6" t="s">
-        <v>243</v>
+        <v>235</v>
       </c>
       <c r="L6" t="s">
-        <v>238</v>
+        <v>230</v>
       </c>
       <c r="M6" t="s">
-        <v>244</v>
+        <v>236</v>
       </c>
       <c r="N6" t="s">
-        <v>254</v>
+        <v>246</v>
       </c>
       <c r="O6" t="s">
-        <v>284</v>
+        <v>276</v>
       </c>
     </row>
     <row r="7" spans="1:15">
@@ -4339,46 +4444,46 @@
         <v>58</v>
       </c>
       <c r="B7" t="s">
-        <v>238</v>
+        <v>230</v>
       </c>
       <c r="C7" t="s">
-        <v>239</v>
+        <v>231</v>
       </c>
       <c r="D7" t="s">
-        <v>238</v>
+        <v>230</v>
       </c>
       <c r="E7" t="s">
-        <v>255</v>
+        <v>247</v>
       </c>
       <c r="F7" t="s">
-        <v>241</v>
+        <v>233</v>
       </c>
       <c r="G7" t="s">
         <v>25</v>
       </c>
       <c r="H7" t="s">
-        <v>246</v>
+        <v>238</v>
       </c>
       <c r="I7" t="s">
-        <v>256</v>
+        <v>248</v>
       </c>
       <c r="J7" t="s">
-        <v>238</v>
+        <v>230</v>
       </c>
       <c r="K7" t="s">
-        <v>243</v>
+        <v>235</v>
       </c>
       <c r="L7" t="s">
-        <v>238</v>
+        <v>230</v>
       </c>
       <c r="M7" t="s">
-        <v>244</v>
+        <v>236</v>
       </c>
       <c r="N7" t="s">
-        <v>245</v>
+        <v>237</v>
       </c>
       <c r="O7" t="s">
-        <v>283</v>
+        <v>275</v>
       </c>
     </row>
     <row r="8" spans="1:15">
@@ -4386,46 +4491,46 @@
         <v>67</v>
       </c>
       <c r="B8" t="s">
+        <v>230</v>
+      </c>
+      <c r="C8" t="s">
+        <v>249</v>
+      </c>
+      <c r="D8" t="s">
         <v>238</v>
       </c>
-      <c r="C8" t="s">
-        <v>257</v>
-      </c>
-      <c r="D8" t="s">
-        <v>246</v>
-      </c>
       <c r="E8" t="s">
-        <v>247</v>
+        <v>239</v>
       </c>
       <c r="F8" t="s">
-        <v>241</v>
+        <v>233</v>
       </c>
       <c r="G8" t="s">
         <v>25</v>
       </c>
       <c r="H8" t="s">
-        <v>246</v>
+        <v>238</v>
       </c>
       <c r="I8" t="s">
-        <v>256</v>
+        <v>248</v>
       </c>
       <c r="J8" t="s">
-        <v>238</v>
+        <v>230</v>
       </c>
       <c r="K8" t="s">
-        <v>243</v>
+        <v>235</v>
       </c>
       <c r="L8" t="s">
-        <v>238</v>
+        <v>230</v>
       </c>
       <c r="M8" t="s">
-        <v>244</v>
+        <v>236</v>
       </c>
       <c r="N8" t="s">
-        <v>245</v>
+        <v>237</v>
       </c>
       <c r="O8" t="s">
-        <v>283</v>
+        <v>275</v>
       </c>
     </row>
     <row r="9" spans="1:15">
@@ -4433,46 +4538,46 @@
         <v>75</v>
       </c>
       <c r="B9" t="s">
+        <v>230</v>
+      </c>
+      <c r="C9" t="s">
+        <v>231</v>
+      </c>
+      <c r="D9" t="s">
         <v>238</v>
       </c>
-      <c r="C9" t="s">
+      <c r="E9" t="s">
         <v>239</v>
       </c>
-      <c r="D9" t="s">
-        <v>246</v>
-      </c>
-      <c r="E9" t="s">
-        <v>247</v>
-      </c>
       <c r="F9" t="s">
-        <v>241</v>
+        <v>233</v>
       </c>
       <c r="G9" t="s">
         <v>25</v>
       </c>
       <c r="H9" t="s">
-        <v>238</v>
+        <v>230</v>
       </c>
       <c r="I9" t="s">
-        <v>258</v>
+        <v>250</v>
       </c>
       <c r="J9" t="s">
-        <v>238</v>
+        <v>230</v>
       </c>
       <c r="K9" t="s">
-        <v>243</v>
+        <v>235</v>
       </c>
       <c r="L9" t="s">
-        <v>238</v>
+        <v>230</v>
       </c>
       <c r="M9" t="s">
-        <v>244</v>
+        <v>236</v>
       </c>
       <c r="N9" t="s">
-        <v>245</v>
+        <v>237</v>
       </c>
       <c r="O9" t="s">
-        <v>283</v>
+        <v>275</v>
       </c>
     </row>
     <row r="10" spans="1:15">
@@ -4480,46 +4585,46 @@
         <v>83</v>
       </c>
       <c r="B10" t="s">
-        <v>238</v>
+        <v>230</v>
       </c>
       <c r="C10" t="s">
-        <v>259</v>
+        <v>251</v>
       </c>
       <c r="D10" t="s">
-        <v>238</v>
+        <v>230</v>
       </c>
       <c r="E10" t="s">
-        <v>240</v>
+        <v>232</v>
       </c>
       <c r="F10" t="s">
-        <v>241</v>
+        <v>233</v>
       </c>
       <c r="G10" t="s">
         <v>25</v>
       </c>
       <c r="H10" t="s">
-        <v>238</v>
+        <v>230</v>
       </c>
       <c r="I10" t="s">
-        <v>258</v>
+        <v>250</v>
       </c>
       <c r="J10" t="s">
-        <v>238</v>
+        <v>230</v>
       </c>
       <c r="K10" t="s">
-        <v>243</v>
+        <v>235</v>
       </c>
       <c r="L10" t="s">
-        <v>238</v>
+        <v>230</v>
       </c>
       <c r="M10" t="s">
-        <v>244</v>
+        <v>236</v>
       </c>
       <c r="N10" t="s">
-        <v>245</v>
+        <v>237</v>
       </c>
       <c r="O10" t="s">
-        <v>283</v>
+        <v>275</v>
       </c>
     </row>
     <row r="11" spans="1:15">
@@ -4527,46 +4632,46 @@
         <v>87</v>
       </c>
       <c r="B11" t="s">
-        <v>238</v>
+        <v>230</v>
       </c>
       <c r="C11" t="s">
-        <v>260</v>
+        <v>252</v>
       </c>
       <c r="D11" t="s">
-        <v>238</v>
+        <v>230</v>
       </c>
       <c r="E11" t="s">
-        <v>252</v>
+        <v>244</v>
       </c>
       <c r="F11" t="s">
-        <v>241</v>
+        <v>233</v>
       </c>
       <c r="G11" t="s">
         <v>25</v>
       </c>
       <c r="H11" t="s">
-        <v>238</v>
+        <v>230</v>
       </c>
       <c r="I11" t="s">
-        <v>261</v>
+        <v>253</v>
       </c>
       <c r="J11" t="s">
-        <v>238</v>
+        <v>230</v>
       </c>
       <c r="K11" t="s">
-        <v>243</v>
+        <v>235</v>
       </c>
       <c r="L11" t="s">
-        <v>238</v>
+        <v>230</v>
       </c>
       <c r="M11" t="s">
-        <v>244</v>
+        <v>236</v>
       </c>
       <c r="N11" t="s">
-        <v>245</v>
+        <v>237</v>
       </c>
       <c r="O11" t="s">
-        <v>283</v>
+        <v>275</v>
       </c>
     </row>
     <row r="12" spans="1:15">
@@ -4574,46 +4679,46 @@
         <v>93</v>
       </c>
       <c r="B12" t="s">
+        <v>230</v>
+      </c>
+      <c r="C12" t="s">
+        <v>231</v>
+      </c>
+      <c r="D12" t="s">
         <v>238</v>
       </c>
-      <c r="C12" t="s">
+      <c r="E12" t="s">
         <v>239</v>
       </c>
-      <c r="D12" t="s">
-        <v>246</v>
-      </c>
-      <c r="E12" t="s">
-        <v>247</v>
-      </c>
       <c r="F12" t="s">
-        <v>241</v>
+        <v>233</v>
       </c>
       <c r="G12" t="s">
         <v>25</v>
       </c>
       <c r="H12" t="s">
-        <v>238</v>
+        <v>230</v>
       </c>
       <c r="I12" t="s">
-        <v>262</v>
+        <v>254</v>
       </c>
       <c r="J12" t="s">
-        <v>238</v>
+        <v>230</v>
       </c>
       <c r="K12" t="s">
-        <v>243</v>
+        <v>235</v>
       </c>
       <c r="L12" t="s">
-        <v>238</v>
+        <v>230</v>
       </c>
       <c r="M12" t="s">
-        <v>244</v>
+        <v>236</v>
       </c>
       <c r="N12" t="s">
-        <v>254</v>
+        <v>246</v>
       </c>
       <c r="O12" t="s">
-        <v>284</v>
+        <v>276</v>
       </c>
     </row>
     <row r="13" spans="1:15">
@@ -4621,46 +4726,46 @@
         <v>97</v>
       </c>
       <c r="B13" t="s">
-        <v>238</v>
+        <v>230</v>
       </c>
       <c r="C13" t="s">
-        <v>239</v>
+        <v>231</v>
       </c>
       <c r="D13" t="s">
-        <v>238</v>
+        <v>230</v>
       </c>
       <c r="E13" t="s">
-        <v>263</v>
+        <v>255</v>
       </c>
       <c r="F13" t="s">
-        <v>241</v>
+        <v>233</v>
       </c>
       <c r="G13" t="s">
         <v>25</v>
       </c>
       <c r="H13" t="s">
-        <v>241</v>
+        <v>233</v>
       </c>
       <c r="I13" t="s">
-        <v>264</v>
+        <v>256</v>
       </c>
       <c r="J13" t="s">
-        <v>238</v>
+        <v>230</v>
       </c>
       <c r="K13" t="s">
-        <v>243</v>
+        <v>235</v>
       </c>
       <c r="L13" t="s">
-        <v>238</v>
+        <v>230</v>
       </c>
       <c r="M13" t="s">
-        <v>244</v>
+        <v>236</v>
       </c>
       <c r="N13" t="s">
-        <v>245</v>
+        <v>237</v>
       </c>
       <c r="O13" t="s">
-        <v>283</v>
+        <v>275</v>
       </c>
     </row>
     <row r="14" spans="1:15">
@@ -4668,46 +4773,46 @@
         <v>104</v>
       </c>
       <c r="B14" t="s">
+        <v>230</v>
+      </c>
+      <c r="C14" t="s">
+        <v>231</v>
+      </c>
+      <c r="D14" t="s">
+        <v>230</v>
+      </c>
+      <c r="E14" t="s">
+        <v>257</v>
+      </c>
+      <c r="F14" t="s">
+        <v>233</v>
+      </c>
+      <c r="G14" t="s">
+        <v>258</v>
+      </c>
+      <c r="H14" t="s">
         <v>238</v>
       </c>
-      <c r="C14" t="s">
-        <v>239</v>
-      </c>
-      <c r="D14" t="s">
-        <v>238</v>
-      </c>
-      <c r="E14" t="s">
-        <v>265</v>
-      </c>
-      <c r="F14" t="s">
-        <v>241</v>
-      </c>
-      <c r="G14" t="s">
-        <v>266</v>
-      </c>
-      <c r="H14" t="s">
-        <v>246</v>
-      </c>
       <c r="I14" t="s">
-        <v>256</v>
+        <v>248</v>
       </c>
       <c r="J14" t="s">
-        <v>238</v>
+        <v>230</v>
       </c>
       <c r="K14" t="s">
-        <v>243</v>
+        <v>235</v>
       </c>
       <c r="L14" t="s">
-        <v>238</v>
+        <v>230</v>
       </c>
       <c r="M14" t="s">
-        <v>244</v>
+        <v>236</v>
       </c>
       <c r="N14" t="s">
-        <v>245</v>
+        <v>237</v>
       </c>
       <c r="O14" t="s">
-        <v>283</v>
+        <v>275</v>
       </c>
     </row>
     <row r="15" spans="1:15">
@@ -4715,46 +4820,46 @@
         <v>111</v>
       </c>
       <c r="B15" t="s">
-        <v>238</v>
+        <v>230</v>
       </c>
       <c r="C15" t="s">
-        <v>239</v>
+        <v>231</v>
       </c>
       <c r="D15" t="s">
-        <v>238</v>
+        <v>230</v>
       </c>
       <c r="E15" t="s">
-        <v>267</v>
+        <v>259</v>
       </c>
       <c r="F15" t="s">
-        <v>241</v>
+        <v>233</v>
       </c>
       <c r="G15" t="s">
         <v>25</v>
       </c>
       <c r="H15" t="s">
-        <v>246</v>
+        <v>238</v>
       </c>
       <c r="I15" t="s">
-        <v>256</v>
+        <v>248</v>
       </c>
       <c r="J15" t="s">
-        <v>238</v>
+        <v>230</v>
       </c>
       <c r="K15" t="s">
-        <v>243</v>
+        <v>235</v>
       </c>
       <c r="L15" t="s">
-        <v>238</v>
+        <v>230</v>
       </c>
       <c r="M15" t="s">
-        <v>244</v>
+        <v>236</v>
       </c>
       <c r="N15" t="s">
-        <v>245</v>
+        <v>237</v>
       </c>
       <c r="O15" t="s">
-        <v>283</v>
+        <v>275</v>
       </c>
     </row>
   </sheetData>
@@ -4783,46 +4888,46 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>261</v>
+      </c>
+      <c r="C1" t="s">
+        <v>260</v>
+      </c>
+      <c r="D1" t="s">
+        <v>262</v>
+      </c>
+      <c r="E1" t="s">
+        <v>263</v>
+      </c>
+      <c r="F1" t="s">
+        <v>264</v>
+      </c>
+      <c r="G1" t="s">
+        <v>265</v>
+      </c>
+      <c r="H1" t="s">
+        <v>266</v>
+      </c>
+      <c r="I1" t="s">
+        <v>267</v>
+      </c>
+      <c r="J1" t="s">
+        <v>268</v>
+      </c>
+      <c r="K1" t="s">
         <v>269</v>
       </c>
-      <c r="C1" t="s">
-        <v>268</v>
-      </c>
-      <c r="D1" t="s">
+      <c r="L1" t="s">
         <v>270</v>
       </c>
-      <c r="E1" t="s">
+      <c r="M1" t="s">
         <v>271</v>
       </c>
-      <c r="F1" t="s">
+      <c r="N1" t="s">
         <v>272</v>
       </c>
-      <c r="G1" t="s">
+      <c r="O1" t="s">
         <v>273</v>
-      </c>
-      <c r="H1" t="s">
-        <v>274</v>
-      </c>
-      <c r="I1" t="s">
-        <v>275</v>
-      </c>
-      <c r="J1" t="s">
-        <v>276</v>
-      </c>
-      <c r="K1" t="s">
-        <v>277</v>
-      </c>
-      <c r="L1" t="s">
-        <v>278</v>
-      </c>
-      <c r="M1" t="s">
-        <v>279</v>
-      </c>
-      <c r="N1" t="s">
-        <v>280</v>
-      </c>
-      <c r="O1" t="s">
-        <v>281</v>
       </c>
     </row>
     <row r="2" spans="1:15">
@@ -4830,46 +4935,46 @@
         <v>119</v>
       </c>
       <c r="B2" t="s">
-        <v>245</v>
+        <v>237</v>
       </c>
       <c r="C2" t="s">
-        <v>285</v>
+        <v>277</v>
       </c>
       <c r="D2" t="s">
-        <v>245</v>
+        <v>237</v>
       </c>
       <c r="E2" t="s">
-        <v>285</v>
+        <v>277</v>
       </c>
       <c r="F2" t="s">
-        <v>245</v>
+        <v>237</v>
       </c>
       <c r="G2" t="s">
-        <v>286</v>
+        <v>278</v>
       </c>
       <c r="H2" t="s">
+        <v>230</v>
+      </c>
+      <c r="I2" t="s">
+        <v>240</v>
+      </c>
+      <c r="J2" t="s">
         <v>238</v>
       </c>
-      <c r="I2" t="s">
-        <v>248</v>
-      </c>
-      <c r="J2" t="s">
-        <v>246</v>
-      </c>
       <c r="K2" t="s">
-        <v>287</v>
+        <v>279</v>
       </c>
       <c r="L2" t="s">
-        <v>238</v>
+        <v>230</v>
       </c>
       <c r="M2" t="s">
-        <v>244</v>
+        <v>236</v>
       </c>
       <c r="N2" t="s">
-        <v>245</v>
+        <v>237</v>
       </c>
       <c r="O2" t="s">
-        <v>288</v>
+        <v>280</v>
       </c>
     </row>
     <row r="3" spans="1:15">
@@ -4877,46 +4982,46 @@
         <v>124</v>
       </c>
       <c r="B3" t="s">
-        <v>238</v>
+        <v>230</v>
       </c>
       <c r="C3" t="s">
-        <v>239</v>
+        <v>231</v>
       </c>
       <c r="D3" t="s">
-        <v>238</v>
+        <v>230</v>
       </c>
       <c r="E3" t="s">
-        <v>289</v>
+        <v>281</v>
       </c>
       <c r="F3" t="s">
-        <v>241</v>
+        <v>233</v>
       </c>
       <c r="G3" t="s">
         <v>25</v>
       </c>
       <c r="H3" t="s">
-        <v>238</v>
+        <v>230</v>
       </c>
       <c r="I3" t="s">
-        <v>248</v>
+        <v>240</v>
       </c>
       <c r="J3" t="s">
-        <v>238</v>
+        <v>230</v>
       </c>
       <c r="K3" t="s">
-        <v>243</v>
+        <v>235</v>
       </c>
       <c r="L3" t="s">
-        <v>238</v>
+        <v>230</v>
       </c>
       <c r="M3" t="s">
-        <v>290</v>
+        <v>282</v>
       </c>
       <c r="N3" t="s">
-        <v>245</v>
+        <v>237</v>
       </c>
       <c r="O3" t="s">
-        <v>283</v>
+        <v>275</v>
       </c>
     </row>
     <row r="4" spans="1:15">
@@ -4924,46 +5029,46 @@
         <v>130</v>
       </c>
       <c r="B4" t="s">
-        <v>238</v>
+        <v>230</v>
       </c>
       <c r="C4" t="s">
-        <v>259</v>
+        <v>251</v>
       </c>
       <c r="D4" t="s">
-        <v>238</v>
+        <v>230</v>
       </c>
       <c r="E4" t="s">
-        <v>289</v>
+        <v>281</v>
       </c>
       <c r="F4" t="s">
-        <v>238</v>
+        <v>230</v>
       </c>
       <c r="G4" t="s">
         <v>134</v>
       </c>
       <c r="H4" t="s">
-        <v>238</v>
+        <v>230</v>
       </c>
       <c r="I4" t="s">
-        <v>291</v>
+        <v>283</v>
       </c>
       <c r="J4" t="s">
-        <v>238</v>
+        <v>230</v>
       </c>
       <c r="K4" t="s">
-        <v>292</v>
+        <v>284</v>
       </c>
       <c r="L4" t="s">
-        <v>238</v>
+        <v>230</v>
       </c>
       <c r="M4" t="s">
-        <v>244</v>
+        <v>236</v>
       </c>
       <c r="N4" t="s">
-        <v>245</v>
+        <v>237</v>
       </c>
       <c r="O4" t="s">
-        <v>283</v>
+        <v>275</v>
       </c>
     </row>
   </sheetData>

</xml_diff>